<commit_message>
Updata Data & PPT & Data
</commit_message>
<xml_diff>
--- a/Doc/Compare_Data.xlsx
+++ b/Doc/Compare_Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5995C65-F140-4E93-81E6-5DD98D8338BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13176524-BB22-490A-8E16-4B163C2C0D3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cleveland_297" sheetId="1" r:id="rId1"/>
@@ -26,41 +26,41 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="24">
   <si>
     <t>Validation</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Classifier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Algorithm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>DR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>AC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>10-fold</t>
   </si>
   <si>
     <t>10-fold</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>SVM</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">10-fold </t>
@@ -70,38 +70,54 @@
   </si>
   <si>
     <t>5nn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1nn</t>
   </si>
   <si>
     <t>Lasso</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>GDFS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>FSFOA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>IFSFOA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Best AC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Acc Delta</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>70%-30%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1nn</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">10-fold </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cart</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -117,25 +133,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="13.5"/>
-      <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,17 +170,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -438,7 +463,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A11" sqref="A11:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -489,23 +514,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>1.3952734470367401</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>7.6923076923076802E-2</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2">
         <v>0.52919540229884998</v>
       </c>
       <c r="G2">
@@ -523,11 +548,11 @@
         <v>0.57195402298850495</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3">
         <v>1.39766025543212</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>7.6923076923076802E-2</v>
       </c>
       <c r="D3" t="s">
@@ -536,7 +561,7 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>0.57517241379310302</v>
       </c>
       <c r="G3">
@@ -554,11 +579,11 @@
         <v>0.61574712643678098</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4">
         <v>0.26223230361938399</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>7.6923076923076802E-2</v>
       </c>
       <c r="D4" t="s">
@@ -567,7 +592,7 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>0.57195402298850495</v>
       </c>
       <c r="G4">
@@ -585,20 +610,20 @@
         <v>0.58517241379310303</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5">
         <v>0.22420382499694799</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>7.6923076923076802E-2</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
+        <v>22</v>
+      </c>
+      <c r="F5">
         <v>0.48471264367816003</v>
       </c>
       <c r="G5">
@@ -616,32 +641,55 @@
         <v>0.53252873563218395</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>115.743476390838</v>
       </c>
       <c r="C7" s="1">
         <v>0.53846153846153799</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1">
         <v>0.57195402298850495</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <f>(N2-F7)/N2*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8">
         <v>109.103744029998</v>
       </c>
       <c r="C8" s="1">
@@ -656,13 +704,13 @@
       <c r="F8" s="1">
         <v>0.61574712643678098</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <f t="shared" ref="G8:G10" si="1">(N3-F8)/N3*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9">
         <v>3.2319221496582</v>
       </c>
       <c r="C9" s="1">
@@ -677,49 +725,72 @@
       <c r="F9" s="1">
         <v>0.58517241379310303</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10">
         <v>1.60746073722839</v>
       </c>
       <c r="C10" s="1">
         <v>0.61538461538461497</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1">
         <v>0.53252873563218395</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>11.3392724990844</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.30769230769230699</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="F12">
         <v>0.49563218390804498</v>
       </c>
       <c r="G12">
@@ -727,11 +798,11 @@
         <v>13.344051446945393</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>10.915215015411301</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0.69230769230769196</v>
       </c>
       <c r="D13" t="s">
@@ -740,7 +811,7 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>0.56574712643678104</v>
       </c>
       <c r="G13">
@@ -748,11 +819,11 @@
         <v>8.120216539107707</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14">
         <v>0.28925752639770502</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>0.53846153846153799</v>
       </c>
       <c r="D14" t="s">
@@ -761,7 +832,7 @@
       <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>0.56839080459770097</v>
       </c>
       <c r="G14">
@@ -769,20 +840,20 @@
         <v>2.8678059320368892</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>8.20744037628173E-2</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.46153846153846101</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
+        <v>22</v>
+      </c>
+      <c r="F15">
         <v>0.52206896551724102</v>
       </c>
       <c r="G15">
@@ -790,23 +861,46 @@
         <v>1.9641700841787919</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>13.0475077629089</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>0.30769230769230699</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="1">
+        <v>20</v>
+      </c>
+      <c r="F17">
         <v>0.51942528735632099</v>
       </c>
       <c r="G17">
@@ -814,11 +908,11 @@
         <v>9.1840836012861971</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="1">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18">
         <v>13.047648191452</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>0.61538461538461497</v>
       </c>
       <c r="D18" t="s">
@@ -827,7 +921,7 @@
       <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
         <v>0.56908045977011401</v>
       </c>
       <c r="G18">
@@ -835,11 +929,11 @@
         <v>7.5788687698339183</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19">
         <v>0.274243354797363</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>0.61538461538461497</v>
       </c>
       <c r="D19" t="s">
@@ -848,7 +942,7 @@
       <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>0.55528735632183901</v>
       </c>
       <c r="G19">
@@ -856,20 +950,20 @@
         <v>5.1070516597917335</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B20" s="1">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20">
         <v>9.8088979721069294E-2</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>0.46153846153846101</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1">
+        <v>22</v>
+      </c>
+      <c r="F20">
         <v>0.49482758620689599</v>
       </c>
       <c r="G20">
@@ -878,7 +972,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -888,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3907598-561C-468A-AF5C-D0D6F3CC7F91}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -935,23 +1029,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>1.38831567764282</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0.29411764705882298</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2">
         <v>0.88055555555555498</v>
       </c>
       <c r="G2">
@@ -969,11 +1063,11 @@
         <v>0.90309523809523795</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3">
         <v>1.3984780311584399</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>0.29411764705882298</v>
       </c>
       <c r="D3" t="s">
@@ -982,7 +1076,7 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>0.84365079365079299</v>
       </c>
       <c r="G3">
@@ -1000,11 +1094,11 @@
         <v>0.89476190476190398</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4">
         <v>0.238202810287475</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>0.29411764705882298</v>
       </c>
       <c r="D4" t="s">
@@ -1016,7 +1110,7 @@
       <c r="F4" s="1">
         <v>0.94595238095237999</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1031,20 +1125,20 @@
         <v>0.94595238095237999</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5">
         <v>0.24121904373168901</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>0.29411764705882298</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
+        <v>22</v>
+      </c>
+      <c r="F5">
         <v>0.88611111111111096</v>
       </c>
       <c r="G5">
@@ -1062,23 +1156,46 @@
         <v>0.89468253968253897</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>110.02384161949099</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>0.64705882352941102</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1">
+        <v>20</v>
+      </c>
+      <c r="F7">
         <v>0.89484126984126999</v>
       </c>
       <c r="G7">
@@ -1086,11 +1203,11 @@
         <v>0.9139643202390042</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8">
         <v>110.034425973892</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>0.64705882352941102</v>
       </c>
       <c r="D8" t="s">
@@ -1099,7 +1216,7 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>0.86619047619047596</v>
       </c>
       <c r="G8">
@@ -1107,11 +1224,11 @@
         <v>3.1931878658860513</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9">
         <v>2.6844332218170099</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>0.35294117647058798</v>
       </c>
       <c r="D9" t="s">
@@ -1120,7 +1237,7 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>0.93452380952380898</v>
       </c>
       <c r="G9">
@@ -1128,44 +1245,67 @@
         <v>1.2081550465642661</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10">
         <v>2.4071874618530198</v>
       </c>
       <c r="C10" s="1">
         <v>0.67647058823529405</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1">
         <v>0.89468253968253897</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>12.5266788005828</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.5</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="F12">
         <v>0.883492063492063</v>
       </c>
       <c r="G12">
@@ -1173,11 +1313,11 @@
         <v>2.1706652605677519</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>13.5132908821105</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0.55882352941176405</v>
       </c>
       <c r="D13" t="s">
@@ -1186,7 +1326,7 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>0.86357142857142799</v>
       </c>
       <c r="G13">
@@ -1194,11 +1334,11 @@
         <v>3.4858967535923173</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14">
         <v>0.18815779685974099</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>0.61764705882352899</v>
       </c>
       <c r="D14" t="s">
@@ -1207,7 +1347,7 @@
       <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>0.92857142857142805</v>
       </c>
       <c r="G14">
@@ -1215,20 +1355,20 @@
         <v>1.8374024666498421</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>0.226205348968505</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.52941176470588203</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
+        <v>22</v>
+      </c>
+      <c r="F15">
         <v>0.87777777777777699</v>
       </c>
       <c r="G15">
@@ -1236,32 +1376,55 @@
         <v>1.8894704160383313</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>65.6905357837677</v>
       </c>
       <c r="C17" s="1">
         <v>0.73529411764705799</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1">
         <v>0.90309523809523795</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <f>(N2-F17)/N2*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="1">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18">
         <v>57.718045473098698</v>
       </c>
       <c r="C18" s="1">
@@ -1276,13 +1439,13 @@
       <c r="F18" s="1">
         <v>0.89476190476190398</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19">
         <v>1.20709133148193</v>
       </c>
       <c r="C19" s="1">
@@ -1294,7 +1457,7 @@
       <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>0.92873015873015796</v>
       </c>
       <c r="G19">
@@ -1302,20 +1465,20 @@
         <v>1.8206225354475862</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B20" s="1">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20">
         <v>1.39827013015747</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>0.61764705882352899</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1">
+        <v>22</v>
+      </c>
+      <c r="F20">
         <v>0.88047619047618997</v>
       </c>
       <c r="G20">
@@ -1324,7 +1487,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1334,7 +1497,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A6" sqref="A6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1380,26 +1543,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>1.28418040275573</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1">
         <v>0.76666666666666605</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <f>(N2-F2)/N2*100</f>
         <v>0</v>
       </c>
@@ -1414,11 +1577,11 @@
         <v>0.76666666666666605</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3">
         <v>1.2931752204895</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
@@ -1430,7 +1593,7 @@
       <c r="F3" s="1">
         <v>0.844444444444444</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <f t="shared" ref="G3:G5" si="0">(N3-F3)/N3*100</f>
         <v>0</v>
       </c>
@@ -1445,11 +1608,11 @@
         <v>0.844444444444444</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4">
         <v>0.139126300811767</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>0</v>
       </c>
       <c r="D4" t="s">
@@ -1458,7 +1621,7 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>0.83333333333333304</v>
       </c>
       <c r="G4">
@@ -1476,20 +1639,20 @@
         <v>0.84074074074074001</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5">
         <v>0.128116369247436</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
+        <v>22</v>
+      </c>
+      <c r="F5">
         <v>0.79259259259259196</v>
       </c>
       <c r="G5">
@@ -1507,23 +1670,46 @@
         <v>0.79629629629629595</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>109.3668820858</v>
       </c>
       <c r="C7" s="1">
         <v>0.69230769230769196</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1">
+        <v>20</v>
+      </c>
+      <c r="F7">
         <v>0.72222222222222199</v>
       </c>
       <c r="G7">
@@ -1531,8 +1717,8 @@
         <v>5.797101449275317</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8">
         <v>109.446511745452</v>
       </c>
       <c r="C8" s="1">
@@ -1544,7 +1730,7 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>0.74444444444444402</v>
       </c>
       <c r="G8">
@@ -1552,8 +1738,8 @@
         <v>11.842105263157897</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9">
         <v>2.3251073360443102</v>
       </c>
       <c r="C9" s="1">
@@ -1565,7 +1751,7 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>0.77037037037037004</v>
       </c>
       <c r="G9">
@@ -1573,20 +1759,20 @@
         <v>8.3700440528633955</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10">
         <v>1.2781610488891599</v>
       </c>
       <c r="C10" s="1">
         <v>0.76923076923076905</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1">
+        <v>22</v>
+      </c>
+      <c r="F10">
         <v>0.718518518518518</v>
       </c>
       <c r="G10">
@@ -1594,23 +1780,46 @@
         <v>9.7674418604651407</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>12.831749677657999</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.30769230769230699</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="F12">
         <v>0.76296296296296195</v>
       </c>
       <c r="G12">
@@ -1618,11 +1827,11 @@
         <v>0.4830917874396653</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>14.2827265262603</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0.53846153846153799</v>
       </c>
       <c r="D13" t="s">
@@ -1631,7 +1840,7 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>0.79629629629629595</v>
       </c>
       <c r="G13">
@@ -1639,11 +1848,11 @@
         <v>5.7017543859649038</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14">
         <v>0.186163425445556</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>0.53846153846153799</v>
       </c>
       <c r="D14" t="s">
@@ -1652,7 +1861,7 @@
       <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>0.81111111111111101</v>
       </c>
       <c r="G14">
@@ -1660,20 +1869,20 @@
         <v>3.5242290748897966</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>8.2066535949707003E-2</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.38461538461538403</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
+        <v>22</v>
+      </c>
+      <c r="F15">
         <v>0.74814814814814801</v>
       </c>
       <c r="G15">
@@ -1681,35 +1890,58 @@
         <v>6.0465116279069528</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>14.3291566371917</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>0.61538461538461497</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1">
         <v>0.76666666666666605</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <f>(N2-F17)/N2*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="1">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18">
         <v>19.015325069427401</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>0.30769230769230699</v>
       </c>
       <c r="D18" t="s">
@@ -1718,7 +1950,7 @@
       <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
         <v>0.82962962962962905</v>
       </c>
       <c r="G18">
@@ -1726,11 +1958,11 @@
         <v>1.7543859649122973</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19">
         <v>0.23221921920776301</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>0.46153846153846101</v>
       </c>
       <c r="D19" t="s">
@@ -1742,34 +1974,34 @@
       <c r="F19" s="1">
         <v>0.84074074074074001</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B20" s="1">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20">
         <v>0.136123657226562</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>0.61538461538461497</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F20" s="1">
         <v>0.79629629629629595</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1779,7 +2011,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A11" sqref="A11:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1825,23 +2057,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>2.52315998077392</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0.27777777777777701</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2">
         <v>0.68184873949579805</v>
       </c>
       <c r="G2">
@@ -1859,11 +2091,11 @@
         <v>0.704397759103641</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3">
         <v>2.83370018005371</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>0.27777777777777701</v>
       </c>
       <c r="D3" t="s">
@@ -1872,7 +2104,7 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>0.71273109243697397</v>
       </c>
       <c r="G3">
@@ -1890,11 +2122,11 @@
         <v>0.73053221288515402</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4">
         <v>1.4573731422424301</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>0.27777777777777701</v>
       </c>
       <c r="D4" t="s">
@@ -1903,7 +2135,7 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>0.76600840336134401</v>
       </c>
       <c r="G4">
@@ -1921,20 +2153,20 @@
         <v>0.76831932773109202</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5">
         <v>1.37127161026</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>0.27777777777777701</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
+        <v>22</v>
+      </c>
+      <c r="F5">
         <v>0.69511204481792699</v>
       </c>
       <c r="G5">
@@ -1952,23 +2184,46 @@
         <v>0.69967787114845903</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>113.056159496307</v>
       </c>
       <c r="C7" s="1">
         <v>0.61111111111111105</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1">
+        <v>20</v>
+      </c>
+      <c r="F7">
         <v>0.70103641456582599</v>
       </c>
       <c r="G7">
@@ -1976,8 +2231,8 @@
         <v>0.47719409869962892</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8">
         <v>113.07759594917199</v>
       </c>
       <c r="C8" s="1">
@@ -1989,7 +2244,7 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>0.69973389355742299</v>
       </c>
       <c r="G8">
@@ -1997,8 +2252,8 @@
         <v>4.2158742331288259</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9">
         <v>13.745487928390499</v>
       </c>
       <c r="C9" s="1">
@@ -2013,61 +2268,84 @@
       <c r="F9" s="1">
         <v>0.76831932773109202</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10">
         <v>5.3788866996765101</v>
       </c>
       <c r="C10" s="1">
         <v>0.5</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F10" s="1">
         <v>0.69967787114845903</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>18.773735284805198</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.44444444444444398</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1">
         <v>0.704397759103641</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <f>(N2-F12)/N2*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>13.8055102825164</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0.38888888888888801</v>
       </c>
       <c r="D13" t="s">
@@ -2076,7 +2354,7 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>0.71155462184873897</v>
       </c>
       <c r="G13">
@@ -2084,11 +2362,11 @@
         <v>2.5977760736196989</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14">
         <v>1.1740648746490401</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>0.27777777777777701</v>
       </c>
       <c r="D14" t="s">
@@ -2097,7 +2375,7 @@
       <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>0.75644257703081197</v>
       </c>
       <c r="G14">
@@ -2105,20 +2383,20 @@
         <v>1.5458091800648872</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>0.265232563018798</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.33333333333333298</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
+        <v>22</v>
+      </c>
+      <c r="F15">
         <v>0.67142857142857104</v>
       </c>
       <c r="G15">
@@ -2126,23 +2404,46 @@
         <v>4.0374722261144651</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>38.473061561584402</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>0.33333333333333298</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="1">
+        <v>20</v>
+      </c>
+      <c r="F17">
         <v>0.68201680672268905</v>
       </c>
       <c r="G17">
@@ -2150,11 +2451,11 @@
         <v>3.1773173738417504</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="1">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18">
         <v>49.387864828109699</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>0.38888888888888801</v>
       </c>
       <c r="D18" t="s">
@@ -2166,16 +2467,16 @@
       <c r="F18" s="1">
         <v>0.73053221288515402</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19">
         <v>3.8384819030761701</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>0.33333333333333298</v>
       </c>
       <c r="D19" t="s">
@@ -2184,7 +2485,7 @@
       <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>0.76598039215686198</v>
       </c>
       <c r="G19">
@@ -2192,20 +2493,20 @@
         <v>0.30442232673452346</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B20" s="1">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20">
         <v>0.892811298370361</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>0.44444444444444398</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1">
+        <v>22</v>
+      </c>
+      <c r="F20">
         <v>0.68668067226890706</v>
       </c>
       <c r="G20">
@@ -2214,7 +2515,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2224,7 +2525,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="A11" sqref="A11:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2270,11 +2571,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>4.2102863788604701</v>
       </c>
       <c r="C2" s="1">
@@ -2284,9 +2585,9 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2">
         <v>0.85</v>
       </c>
       <c r="G2">
@@ -2304,8 +2605,8 @@
         <v>0.94736842105263097</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3">
         <v>4.2344846725463796</v>
       </c>
       <c r="C3" s="1">
@@ -2317,7 +2618,7 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>0.85576923076922995</v>
       </c>
       <c r="G3">
@@ -2335,8 +2636,8 @@
         <v>0.94736842105263097</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4">
         <v>3.0740082263946502</v>
       </c>
       <c r="C4" s="1">
@@ -2348,7 +2649,7 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>0.93012820512820504</v>
       </c>
       <c r="G4">
@@ -2366,8 +2667,8 @@
         <v>0.94736842105263097</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5">
         <v>3.07286047935485</v>
       </c>
       <c r="C5" s="1">
@@ -2377,9 +2678,9 @@
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
+        <v>22</v>
+      </c>
+      <c r="F5">
         <v>0.76987179487179402</v>
       </c>
       <c r="G5">
@@ -2397,23 +2698,46 @@
         <v>0.92105263157894701</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>111.47756743431</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>0.57741935483870899</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1">
+        <v>20</v>
+      </c>
+      <c r="F7">
         <v>0.78947368421052599</v>
       </c>
       <c r="G7">
@@ -2421,11 +2745,11 @@
         <v>16.666666666666647</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8">
         <v>111.56951546669001</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>0.49354838709677401</v>
       </c>
       <c r="D8" t="s">
@@ -2434,7 +2758,7 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>0.55263157894736803</v>
       </c>
       <c r="G8">
@@ -2442,11 +2766,11 @@
         <v>41.666666666666671</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9">
         <v>3.8955338001251198</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>0.34193548387096701</v>
       </c>
       <c r="D9" t="s">
@@ -2455,7 +2779,7 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>0.81578947368420995</v>
       </c>
       <c r="G9">
@@ -2463,20 +2787,20 @@
         <v>13.888888888888895</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10">
         <v>5.9524085521697998</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>0.57419354838709602</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1">
+        <v>22</v>
+      </c>
+      <c r="F10">
         <v>0.84210526315789402</v>
       </c>
       <c r="G10">
@@ -2484,23 +2808,46 @@
         <v>8.5714285714286138</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>11.0098829269409</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.54838709677419295</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="F12">
         <v>0.84210526315789402</v>
       </c>
       <c r="G12">
@@ -2508,11 +2855,11 @@
         <v>11.11111111111113</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>13.8202545642852</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0.47096774193548302</v>
       </c>
       <c r="D13" t="s">
@@ -2521,7 +2868,7 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>0.92105263157894701</v>
       </c>
       <c r="G13">
@@ -2529,11 +2876,11 @@
         <v>2.7777777777777528</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14">
         <v>0.29825687408447199</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>0.48064516129032198</v>
       </c>
       <c r="D14" t="s">
@@ -2545,25 +2892,25 @@
       <c r="F14" s="1">
         <v>0.94736842105263097</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>0.408370971679687</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.49677419354838698</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
+        <v>22</v>
+      </c>
+      <c r="F15">
         <v>0.89473684210526305</v>
       </c>
       <c r="G15">
@@ -2571,35 +2918,58 @@
         <v>2.857142857142831</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>920.24537467956497</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>0.57741935483870899</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1">
         <v>0.94736842105263097</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <f>(N2-F17)/N2*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="1">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18">
         <v>870.95313930511395</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>0.57741935483870899</v>
       </c>
       <c r="D18" t="s">
@@ -2611,16 +2981,16 @@
       <c r="F18" s="1">
         <v>0.94736842105263097</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19">
         <v>18.957506179809499</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>0.62903225806451601</v>
       </c>
       <c r="D19" t="s">
@@ -2632,34 +3002,34 @@
       <c r="F19" s="1">
         <v>0.94736842105263097</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B20" s="1">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20">
         <v>32.222971916198702</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>0.532258064516129</v>
       </c>
       <c r="D20" t="s">
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F20" s="1">
         <v>0.92105263157894701</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2669,7 +3039,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2715,11 +3085,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>21.328305721282899</v>
       </c>
       <c r="C2" s="1">
@@ -2729,9 +3099,9 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2">
         <v>0.73684210526315697</v>
       </c>
       <c r="G2">
@@ -2749,8 +3119,8 @@
         <v>0.94736842105263097</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3">
         <v>21.149477481841998</v>
       </c>
       <c r="C3" s="1">
@@ -2762,7 +3132,7 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>0.68421052631578905</v>
       </c>
       <c r="G3">
@@ -2780,8 +3150,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4">
         <v>20.286529064178399</v>
       </c>
       <c r="C4" s="1">
@@ -2793,7 +3163,7 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>0.73684210526315697</v>
       </c>
       <c r="G4">
@@ -2811,8 +3181,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5">
         <v>20.078588247299098</v>
       </c>
       <c r="C5" s="1">
@@ -2822,14 +3192,14 @@
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1">
+        <v>22</v>
+      </c>
+      <c r="F5">
         <v>0.68421052631578905</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>23.52941176470592</v>
+        <v>27.777777777777779</v>
       </c>
       <c r="L5" t="s">
         <v>9</v>
@@ -2839,38 +3209,61 @@
       </c>
       <c r="N5">
         <f>MAX(F5, F10, F15, F20)</f>
-        <v>0.89473684210526305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+        <v>0.94736842105263097</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>112.95495748519799</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>0.67461005199306701</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F7" s="1">
         <v>0.94736842105263097</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <f>(N2-F7)/N2*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8">
         <v>113.038189649581</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>0.67461005199306701</v>
       </c>
       <c r="D8" t="s">
@@ -2882,16 +3275,16 @@
       <c r="F8" s="1">
         <v>1</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <f t="shared" ref="G8:G10" si="1">(N3-F8)/N3*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9">
         <v>8.5047273635864205</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>0.67461005199306701</v>
       </c>
       <c r="D9" t="s">
@@ -2900,7 +3293,7 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>0.94736842105263097</v>
       </c>
       <c r="G9">
@@ -2908,44 +3301,67 @@
         <v>5.2631578947369029</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10">
         <v>10.6006314754486</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>0.67461005199306701</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1">
+        <v>22</v>
+      </c>
+      <c r="F10">
         <v>0.89473684210526305</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+        <v>5.5555555555555056</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>10.151315212249701</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.49566724436741699</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1">
+        <v>20</v>
+      </c>
+      <c r="F12">
         <v>0.89473684210526305</v>
       </c>
       <c r="G12">
@@ -2953,11 +3369,11 @@
         <v>5.5555555555555056</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>11.6274077892303</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0.52079722703639497</v>
       </c>
       <c r="D13" t="s">
@@ -2966,7 +3382,7 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>0.89473684210526305</v>
       </c>
       <c r="G13">
@@ -2974,11 +3390,11 @@
         <v>10.526315789473696</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14">
         <v>1.3812491893768299</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>0.50043327556325801</v>
       </c>
       <c r="D14" t="s">
@@ -2990,57 +3406,86 @@
       <c r="F14" s="1">
         <v>1</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>1.5153768062591499</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.50909878682842202</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
+        <v>22</v>
+      </c>
+      <c r="F15">
         <v>0.84210526315789402</v>
       </c>
       <c r="G15">
         <f t="shared" si="2"/>
-        <v>5.8823529411765394</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="17.5" x14ac:dyDescent="0.3">
+        <v>11.11111111111113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>2564.6809816360401</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>0.56499133448873395</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1">
         <v>0.94736842105263097</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <f>(N2-F17)/N2*100</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>6099.0280644893601</v>
+      </c>
+      <c r="C18">
+        <v>0.59748700173310199</v>
+      </c>
       <c r="D18" t="s">
         <v>19</v>
       </c>
@@ -3048,46 +3493,59 @@
         <v>11</v>
       </c>
       <c r="F18">
-        <v>0.69047619047619002</v>
+        <v>0.94736842105263097</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
-        <v>30.952380952380999</v>
+        <v>5.2631578947369029</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>561.18020677566506</v>
+      </c>
+      <c r="C19">
+        <v>0.64904679376083196</v>
+      </c>
       <c r="D19" t="s">
         <v>19</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="F19">
-        <v>0.669047619047619</v>
-      </c>
-      <c r="G19">
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>33.095238095238102</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>711.095648050308</v>
+      </c>
+      <c r="C20">
+        <v>0.65424610051993004</v>
+      </c>
       <c r="D20" t="s">
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20">
-        <v>0.75952380952380905</v>
-      </c>
-      <c r="G20">
+        <v>22</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.94736842105263097</v>
+      </c>
+      <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>15.112044817927215</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3096,7 +3554,7 @@
   <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3142,11 +3600,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>415.93556237220702</v>
       </c>
       <c r="C2" s="1">
@@ -3156,9 +3614,9 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2">
         <v>0.8</v>
       </c>
       <c r="G2">
@@ -3176,8 +3634,8 @@
         <v>0.88333333333333297</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3">
         <v>379.95642280578602</v>
       </c>
       <c r="C3" s="1">
@@ -3189,7 +3647,7 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3">
         <v>0.81666666666666599</v>
       </c>
       <c r="G3">
@@ -3207,8 +3665,8 @@
         <v>0.86666666666666603</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4">
         <v>422.91982841491699</v>
       </c>
       <c r="C4" s="1">
@@ -3223,7 +3681,7 @@
       <c r="F4" s="1">
         <v>0.96666666666666601</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3238,8 +3696,8 @@
         <v>0.96666666666666601</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5">
         <v>375.75324440002402</v>
       </c>
       <c r="C5" s="1">
@@ -3249,12 +3707,12 @@
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1">
         <v>0.8</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3269,23 +3727,46 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>398.66558527946398</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>0.43589999999999901</v>
       </c>
       <c r="D7" t="s">
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1">
+        <v>20</v>
+      </c>
+      <c r="F7">
         <v>0.73333333333333295</v>
       </c>
       <c r="G7">
@@ -3293,11 +3774,11 @@
         <v>16.981132075471709</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8">
         <v>399.23260307312</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>0.59419999999999995</v>
       </c>
       <c r="D8" t="s">
@@ -3306,7 +3787,7 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8">
         <v>0.78333333333333299</v>
       </c>
       <c r="G8">
@@ -3314,11 +3795,11 @@
         <v>9.6153846153845883</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9">
         <v>338.36082291602997</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>0.87780000000000002</v>
       </c>
       <c r="D9" t="s">
@@ -3327,7 +3808,7 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>0.7</v>
       </c>
       <c r="G9">
@@ -3335,20 +3816,20 @@
         <v>27.58620689655168</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10">
         <v>342.78976869583101</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>0.76380000000000003</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1">
+        <v>22</v>
+      </c>
+      <c r="F10">
         <v>0.7</v>
       </c>
       <c r="G10">
@@ -3356,35 +3837,58 @@
         <v>12.500000000000011</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>21.512185335159302</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.49759999999999999</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1">
         <v>0.88333333333333297</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <f>(N2-F12)/N2*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="1">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13">
         <v>17.064989328384399</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0.50549999999999995</v>
       </c>
       <c r="D13" t="s">
@@ -3396,16 +3900,16 @@
       <c r="F13" s="1">
         <v>0.86666666666666603</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <f t="shared" ref="G13:G15" si="2">(N3-F13)/N3*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="1">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14">
         <v>15.005628824234</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>0.49419999999999997</v>
       </c>
       <c r="D14" t="s">
@@ -3414,7 +3918,7 @@
       <c r="E14" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>0.8</v>
       </c>
       <c r="G14">
@@ -3422,20 +3926,20 @@
         <v>17.241379310344769</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="17.5" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>14.5131869316101</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.48919999999999902</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1">
+        <v>22</v>
+      </c>
+      <c r="F15">
         <v>0.7</v>
       </c>
       <c r="G15">
@@ -3443,31 +3947,60 @@
         <v>12.500000000000011</v>
       </c>
     </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>24.820551395416199</v>
-      </c>
-      <c r="C17">
-        <v>0.46153846153846101</v>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
       </c>
       <c r="D17" t="s">
         <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F17">
-        <v>0.558965517241379</v>
+        <v>0</v>
       </c>
       <c r="G17">
         <f>(N2-F17)/N2*100</f>
-        <v>36.720884840598579</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
       <c r="D18" t="s">
         <v>19</v>
       </c>
@@ -3475,14 +4008,20 @@
         <v>11</v>
       </c>
       <c r="F18">
-        <v>0.57241379310344798</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
-        <v>33.952254641909803</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
       <c r="D19" t="s">
         <v>19</v>
       </c>
@@ -3490,30 +4029,36 @@
         <v>8</v>
       </c>
       <c r="F19">
-        <v>0.55839080459770096</v>
+        <v>0</v>
       </c>
       <c r="G19">
         <f t="shared" si="3"/>
-        <v>42.235434007134344</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
       <c r="D20" t="s">
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F20">
-        <v>0.49183908045976998</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <f t="shared" si="3"/>
-        <v>38.520114942528757</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Excel & PPT
</commit_message>
<xml_diff>
--- a/Doc/Compare_Data.xlsx
+++ b/Doc/Compare_Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE3F0D9-F409-4E96-8242-67763CA3DE8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F85548D-A1EE-4C4A-8C84-C2DE4F84C3EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cleveland_297" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="26">
   <si>
     <t>Validation</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -117,6 +117,14 @@
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EFSFOA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LassoGA</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -460,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -544,7 +552,7 @@
         <v>12</v>
       </c>
       <c r="N2">
-        <f>MAX(F2, F7, F12, F17)</f>
+        <f>MAX(F2, F7, F12, F17, F22, F27)</f>
         <v>0.57195402298850495</v>
       </c>
     </row>
@@ -575,7 +583,7 @@
         <v>11</v>
       </c>
       <c r="N3">
-        <f>MAX(F3, F8, F13, F18)</f>
+        <f>MAX(F3, F8, F13, F18, F23, F28)</f>
         <v>0.61574712643678098</v>
       </c>
     </row>
@@ -606,7 +614,7 @@
         <v>8</v>
       </c>
       <c r="N4">
-        <f>MAX(F4, F9, F14, F19)</f>
+        <f t="shared" ref="N3:N5" si="1">MAX(F4, F9, F14, F19, F24, F29)</f>
         <v>0.58517241379310303</v>
       </c>
     </row>
@@ -637,7 +645,7 @@
         <v>10</v>
       </c>
       <c r="N5">
-        <f>MAX(F5, F10, F15, F20)</f>
+        <f t="shared" si="1"/>
         <v>0.53252873563218395</v>
       </c>
     </row>
@@ -692,7 +700,7 @@
       <c r="B8">
         <v>109.103744029998</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>0.61538461538461497</v>
       </c>
       <c r="D8" t="s">
@@ -705,7 +713,7 @@
         <v>0.61574712643678098</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G10" si="1">(N3-F8)/N3*100</f>
+        <f t="shared" ref="G8:G10" si="2">(N3-F8)/N3*100</f>
         <v>0</v>
       </c>
     </row>
@@ -726,7 +734,7 @@
         <v>0.58517241379310303</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -747,7 +755,7 @@
         <v>0.53252873563218395</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -802,7 +810,7 @@
       <c r="B13">
         <v>10.915215015411301</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>0.69230769230769196</v>
       </c>
       <c r="D13" t="s">
@@ -815,7 +823,7 @@
         <v>0.56574712643678104</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G15" si="2">(N3-F13)/N3*100</f>
+        <f t="shared" ref="G13:G15" si="3">(N3-F13)/N3*100</f>
         <v>8.120216539107707</v>
       </c>
     </row>
@@ -836,7 +844,7 @@
         <v>0.56839080459770097</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.8678059320368892</v>
       </c>
     </row>
@@ -857,7 +865,7 @@
         <v>0.52206896551724102</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.9641700841787919</v>
       </c>
     </row>
@@ -925,7 +933,7 @@
         <v>0.56908045977011401</v>
       </c>
       <c r="G18">
-        <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
+        <f t="shared" ref="G18:G20" si="4">(N3-F18)/N3*100</f>
         <v>7.5788687698339183</v>
       </c>
     </row>
@@ -933,7 +941,7 @@
       <c r="B19">
         <v>0.274243354797363</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>0.61538461538461497</v>
       </c>
       <c r="D19" t="s">
@@ -946,7 +954,7 @@
         <v>0.55528735632183901</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.1070516597917335</v>
       </c>
     </row>
@@ -967,8 +975,204 @@
         <v>0.49482758620689599</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.0796460176992273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>(N2-F22)/N2*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G25" si="5">(N3-F23)/N3*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>2.4392161369323699</v>
+      </c>
+      <c r="C27">
+        <v>0.23076923076923</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>0.53896551724137898</v>
+      </c>
+      <c r="G27">
+        <f>(N2-F27)/N2*100</f>
+        <v>5.7676848874597342</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>2.2280247211456299</v>
+      </c>
+      <c r="C28">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <v>0.58896551724137902</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:G30" si="6">(N3-F28)/N3*100</f>
+        <v>4.3494493186484462</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>2.23503065109252</v>
+      </c>
+      <c r="C29">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29">
+        <v>0.54494252873563198</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="6"/>
+        <v>6.8748772343350693</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>2.5012722015380802</v>
+      </c>
+      <c r="C30">
+        <v>0.61538461538461497</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30">
+        <v>0.49172413793103398</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="6"/>
+        <v>7.6624217569610336</v>
       </c>
     </row>
   </sheetData>
@@ -980,10 +1184,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3907598-561C-468A-AF5C-D0D6F3CC7F91}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="A6:G10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1059,7 +1263,7 @@
         <v>12</v>
       </c>
       <c r="N2">
-        <f>MAX(F2, F7, F12, F17)</f>
+        <f>MAX(F2, F7, F12, F17, F22, F27)</f>
         <v>0.90309523809523795</v>
       </c>
     </row>
@@ -1090,7 +1294,7 @@
         <v>11</v>
       </c>
       <c r="N3">
-        <f>MAX(F3, F8, F13, F18)</f>
+        <f>MAX(F3, F8, F13, F18, F23, F28)</f>
         <v>0.89476190476190398</v>
       </c>
     </row>
@@ -1107,12 +1311,12 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>0.94595238095237999</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.29278902459430067</v>
       </c>
       <c r="L4" t="s">
         <v>7</v>
@@ -1121,8 +1325,8 @@
         <v>8</v>
       </c>
       <c r="N4">
-        <f>MAX(F4, F9, F14, F19)</f>
-        <v>0.94595238095237999</v>
+        <f t="shared" ref="N4:N5" si="1">MAX(F4, F9, F14, F19, F24, F29)</f>
+        <v>0.94873015873015798</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -1152,7 +1356,7 @@
         <v>10</v>
       </c>
       <c r="N5">
-        <f>MAX(F5, F10, F15, F20)</f>
+        <f t="shared" si="1"/>
         <v>0.89468253968253897</v>
       </c>
     </row>
@@ -1220,7 +1424,7 @@
         <v>0.86619047619047596</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G10" si="1">(N3-F8)/N3*100</f>
+        <f t="shared" ref="G8:G10" si="2">(N3-F8)/N3*100</f>
         <v>3.1931878658860513</v>
       </c>
     </row>
@@ -1241,8 +1445,8 @@
         <v>0.93452380952380898</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
-        <v>1.2081550465642661</v>
+        <f t="shared" si="2"/>
+        <v>1.4974067257821444</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1262,7 +1466,7 @@
         <v>0.89468253968253897</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1330,7 +1534,7 @@
         <v>0.86357142857142799</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G15" si="2">(N3-F13)/N3*100</f>
+        <f t="shared" ref="G13:G15" si="3">(N3-F13)/N3*100</f>
         <v>3.4858967535923173</v>
       </c>
     </row>
@@ -1351,8 +1555,8 @@
         <v>0.92857142857142805</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
-        <v>1.8374024666498421</v>
+        <f t="shared" si="3"/>
+        <v>2.1248117784841671</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1372,7 +1576,7 @@
         <v>0.87777777777777699</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8894704160383313</v>
       </c>
     </row>
@@ -1440,7 +1644,7 @@
         <v>0.89476190476190398</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
+        <f t="shared" ref="G18:G20" si="4">(N3-F18)/N3*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1461,8 +1665,8 @@
         <v>0.92873015873015796</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
-        <v>1.8206225354475862</v>
+        <f t="shared" si="4"/>
+        <v>2.1080809770788056</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1482,8 +1686,204 @@
         <v>0.88047619047618997</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.5878648097223236</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>(N2-F22)/N2*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G25" si="5">(N3-F23)/N3*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>4.2168328762054399</v>
+      </c>
+      <c r="C27">
+        <v>0.47058823529411697</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>0.89761904761904698</v>
+      </c>
+      <c r="G27">
+        <f>(N2-F27)/N2*100</f>
+        <v>0.60638017400480004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>3.1728813648223801</v>
+      </c>
+      <c r="C28">
+        <v>0.52941176470588203</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <v>0.87206349206349199</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:G30" si="6">(N3-F28)/N3*100</f>
+        <v>2.5368103601205552</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>6.1375765800476003</v>
+      </c>
+      <c r="C29">
+        <v>0.47058823529411697</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.94873015873015798</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>3.1418547630310001</v>
+      </c>
+      <c r="C30">
+        <v>0.61764705882352899</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30">
+        <v>0.88880952380952305</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="6"/>
+        <v>0.65643573139360101</v>
       </c>
     </row>
   </sheetData>
@@ -1494,10 +1894,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F238B875-C88B-44D7-86CD-CE4C5F44C54D}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:G10"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1573,7 +1973,7 @@
         <v>12</v>
       </c>
       <c r="N2">
-        <f>MAX(F2, F7, F12, F17)</f>
+        <f>MAX(F2, F7, F12, F17, F22, F27)</f>
         <v>0.76666666666666605</v>
       </c>
     </row>
@@ -1604,7 +2004,7 @@
         <v>11</v>
       </c>
       <c r="N3">
-        <f>MAX(F3, F8, F13, F18)</f>
+        <f>MAX(F3, F8, F13, F18, F23, F28)</f>
         <v>0.844444444444444</v>
       </c>
     </row>
@@ -1626,7 +2026,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>0.88105726872241619</v>
+        <v>1.7467248908297102</v>
       </c>
       <c r="L4" t="s">
         <v>7</v>
@@ -1635,8 +2035,8 @@
         <v>8</v>
       </c>
       <c r="N4">
-        <f>MAX(F4, F9, F14, F19)</f>
-        <v>0.84074074074074001</v>
+        <f t="shared" ref="N4:N5" si="1">MAX(F4, F9, F14, F19, F24, F29)</f>
+        <v>0.84814814814814798</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -1666,7 +2066,7 @@
         <v>10</v>
       </c>
       <c r="N5">
-        <f>MAX(F5, F10, F15, F20)</f>
+        <f t="shared" si="1"/>
         <v>0.79629629629629595</v>
       </c>
     </row>
@@ -1734,7 +2134,7 @@
         <v>0.74444444444444402</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G10" si="1">(N3-F8)/N3*100</f>
+        <f t="shared" ref="G8:G10" si="2">(N3-F8)/N3*100</f>
         <v>11.842105263157897</v>
       </c>
     </row>
@@ -1755,8 +2155,8 @@
         <v>0.77037037037037004</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
-        <v>8.3700440528633955</v>
+        <f t="shared" si="2"/>
+        <v>9.1703056768559161</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1776,7 +2176,7 @@
         <v>0.718518518518518</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.7674418604651407</v>
       </c>
     </row>
@@ -1844,7 +2244,7 @@
         <v>0.79629629629629595</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G15" si="2">(N3-F13)/N3*100</f>
+        <f t="shared" ref="G13:G15" si="3">(N3-F13)/N3*100</f>
         <v>5.7017543859649038</v>
       </c>
     </row>
@@ -1865,8 +2265,8 @@
         <v>0.81111111111111101</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
-        <v>3.5242290748897966</v>
+        <f t="shared" si="3"/>
+        <v>4.36681222707423</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1886,7 +2286,7 @@
         <v>0.74814814814814801</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.0465116279069528</v>
       </c>
     </row>
@@ -1954,7 +2354,7 @@
         <v>0.82962962962962905</v>
       </c>
       <c r="G18">
-        <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
+        <f t="shared" ref="G18:G20" si="4">(N3-F18)/N3*100</f>
         <v>1.7543859649122973</v>
       </c>
     </row>
@@ -1971,12 +2371,12 @@
       <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>0.84074074074074001</v>
       </c>
-      <c r="G19" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="G19">
+        <f t="shared" si="4"/>
+        <v>0.87336244541491403</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1996,8 +2396,204 @@
         <v>0.79629629629629595</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>(N2-F22)/N2*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G25" si="5">(N3-F23)/N3*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>1.82966208457946</v>
+      </c>
+      <c r="C27">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.76666666666666605</v>
+      </c>
+      <c r="G27" s="1">
+        <f>(N2-F27)/N2*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>1.87069988250732</v>
+      </c>
+      <c r="C28">
+        <v>0.38461538461538403</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <v>0.81481481481481399</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:G30" si="6">(N3-F28)/N3*100</f>
+        <v>3.5087719298246078</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>1.7976336479187001</v>
+      </c>
+      <c r="C29">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.84814814814814798</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>1.8406729698181099</v>
+      </c>
+      <c r="C30">
+        <v>0.46153846153846101</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30">
+        <v>0.75925925925925897</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="6"/>
+        <v>4.6511627906976694</v>
       </c>
     </row>
   </sheetData>
@@ -2008,10 +2604,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F83066-A23D-4631-A8C0-781E63CCC626}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2087,7 +2683,7 @@
         <v>12</v>
       </c>
       <c r="N2">
-        <f>MAX(F2, F7, F12, F17)</f>
+        <f>MAX(F2, F7, F12, F17, F22, F27)</f>
         <v>0.704397759103641</v>
       </c>
     </row>
@@ -2118,7 +2714,7 @@
         <v>11</v>
       </c>
       <c r="N3">
-        <f>MAX(F3, F8, F13, F18)</f>
+        <f>MAX(F3, F8, F13, F18, F23, F28)</f>
         <v>0.73053221288515402</v>
       </c>
     </row>
@@ -2140,7 +2736,7 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>0.30077655036641404</v>
+        <v>0.75666848121940866</v>
       </c>
       <c r="L4" t="s">
         <v>7</v>
@@ -2149,8 +2745,8 @@
         <v>8</v>
       </c>
       <c r="N4">
-        <f>MAX(F4, F9, F14, F19)</f>
-        <v>0.76831932773109202</v>
+        <f t="shared" ref="N4:N5" si="1">MAX(F4, F9, F14, F19, F24, F29)</f>
+        <v>0.77184873949579802</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -2171,7 +2767,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0.65256120263424122</v>
+        <v>2.4605467444922313</v>
       </c>
       <c r="L5" t="s">
         <v>9</v>
@@ -2180,8 +2776,8 @@
         <v>10</v>
       </c>
       <c r="N5">
-        <f>MAX(F5, F10, F15, F20)</f>
-        <v>0.69967787114845903</v>
+        <f t="shared" si="1"/>
+        <v>0.71264705882352897</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -2248,7 +2844,7 @@
         <v>0.69973389355742299</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G10" si="1">(N3-F8)/N3*100</f>
+        <f t="shared" ref="G8:G10" si="2">(N3-F8)/N3*100</f>
         <v>4.2158742331288259</v>
       </c>
     </row>
@@ -2265,12 +2861,12 @@
       <c r="E9" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9">
         <v>0.76831932773109202</v>
       </c>
-      <c r="G9" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>0.45726728361460478</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -2286,12 +2882,12 @@
       <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>0.69967787114845903</v>
       </c>
-      <c r="G10" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>1.8198612503193485</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -2358,7 +2954,7 @@
         <v>0.71155462184873897</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G15" si="2">(N3-F13)/N3*100</f>
+        <f t="shared" ref="G13:G15" si="3">(N3-F13)/N3*100</f>
         <v>2.5977760736196989</v>
       </c>
     </row>
@@ -2379,8 +2975,8 @@
         <v>0.75644257703081197</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
-        <v>1.5458091800648872</v>
+        <f t="shared" si="3"/>
+        <v>1.996007984031944</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -2400,8 +2996,8 @@
         <v>0.67142857142857104</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
-        <v>4.0374722261144651</v>
+        <f t="shared" si="3"/>
+        <v>5.7838570838983507</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -2468,7 +3064,7 @@
         <v>0.73053221288515402</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
+        <f t="shared" ref="G18:G20" si="4">(N3-F18)/N3*100</f>
         <v>0</v>
       </c>
     </row>
@@ -2489,8 +3085,8 @@
         <v>0.76598039215686198</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
-        <v>0.30442232673452346</v>
+        <f t="shared" si="4"/>
+        <v>0.76029758664495295</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -2510,8 +3106,204 @@
         <v>0.68668067226890706</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
-        <v>1.857597533879159</v>
+        <f t="shared" si="4"/>
+        <v>3.6436530864925527</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>(N2-F22)/N2*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G25" si="5">(N3-F23)/N3*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>47.678319931030202</v>
+      </c>
+      <c r="C27">
+        <v>0.22222222222222199</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>0.69495798319327695</v>
+      </c>
+      <c r="G27">
+        <f>(N2-F27)/N2*100</f>
+        <v>1.3401200938481594</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>59.008615970611501</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.44444444444444398</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <v>0.71156862745098004</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:G30" si="6">(N3-F28)/N3*100</f>
+        <v>2.5958588957055642</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>62.341644048690704</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.38888888888888801</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.77184873949579802</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>103.141715049743</v>
+      </c>
+      <c r="C30">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.71264705882352897</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2522,10 +3314,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE6E0A8-C326-4938-968A-22A566DDA48F}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:B18"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -2578,7 +3370,7 @@
       <c r="B2">
         <v>4.2102863788604701</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0.880645161290322</v>
       </c>
       <c r="D2" t="s">
@@ -2601,7 +3393,7 @@
         <v>12</v>
       </c>
       <c r="N2">
-        <f>MAX(F2, F7, F12, F17)</f>
+        <f>MAX(F2, F7, F12, F17, F22, F27)</f>
         <v>0.94736842105263097</v>
       </c>
     </row>
@@ -2609,7 +3401,7 @@
       <c r="B3">
         <v>4.2344846725463796</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>0.880645161290322</v>
       </c>
       <c r="D3" t="s">
@@ -2623,7 +3415,7 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G5" si="0">(N3-F3)/N3*100</f>
-        <v>9.6688034188034475</v>
+        <v>12.110187110187127</v>
       </c>
       <c r="L3" t="s">
         <v>7</v>
@@ -2632,15 +3424,15 @@
         <v>11</v>
       </c>
       <c r="N3">
-        <f>MAX(F3, F8, F13, F18)</f>
-        <v>0.94736842105263097</v>
+        <f>MAX(F3, F8, F13, F18, F23, F28)</f>
+        <v>0.97368421052631504</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>3.0740082263946502</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>0.880645161290322</v>
       </c>
       <c r="D4" t="s">
@@ -2663,7 +3455,7 @@
         <v>8</v>
       </c>
       <c r="N4">
-        <f>MAX(F4, F9, F14, F19)</f>
+        <f t="shared" ref="N4:N5" si="1">MAX(F4, F9, F14, F19, F24, F29)</f>
         <v>0.94736842105263097</v>
       </c>
     </row>
@@ -2671,7 +3463,7 @@
       <c r="B5">
         <v>3.07286047935485</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>0.880645161290322</v>
       </c>
       <c r="D5" t="s">
@@ -2694,7 +3486,7 @@
         <v>10</v>
       </c>
       <c r="N5">
-        <f>MAX(F5, F10, F15, F20)</f>
+        <f t="shared" si="1"/>
         <v>0.92105263157894701</v>
       </c>
     </row>
@@ -2762,8 +3554,8 @@
         <v>0.55263157894736803</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G10" si="1">(N3-F8)/N3*100</f>
-        <v>41.666666666666671</v>
+        <f t="shared" ref="G8:G10" si="2">(N3-F8)/N3*100</f>
+        <v>43.243243243243242</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -2783,7 +3575,7 @@
         <v>0.81578947368420995</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.888888888888895</v>
       </c>
     </row>
@@ -2804,7 +3596,7 @@
         <v>0.84210526315789402</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.5714285714286138</v>
       </c>
     </row>
@@ -2872,8 +3664,8 @@
         <v>0.92105263157894701</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G15" si="2">(N3-F13)/N3*100</f>
-        <v>2.7777777777777528</v>
+        <f t="shared" ref="G13:G15" si="3">(N3-F13)/N3*100</f>
+        <v>5.4054054054053697</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -2893,7 +3685,7 @@
         <v>0.94736842105263097</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -2914,7 +3706,7 @@
         <v>0.89473684210526305</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.857142857142831</v>
       </c>
     </row>
@@ -2978,12 +3770,12 @@
       <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18">
         <v>0.94736842105263097</v>
       </c>
-      <c r="G18" s="1">
-        <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
-        <v>0</v>
+      <c r="G18">
+        <f t="shared" ref="G18:G20" si="4">(N3-F18)/N3*100</f>
+        <v>2.7027027027026902</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -3003,7 +3795,7 @@
         <v>0.94736842105263097</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3024,8 +3816,204 @@
         <v>0.92105263157894701</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>(N2-F22)/N2*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G25" si="5">(N3-F23)/N3*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>52.689874410629201</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.90645161290322496</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>0.92105263157894701</v>
+      </c>
+      <c r="G27">
+        <f>(N2-F27)/N2*100</f>
+        <v>2.7777777777777528</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>75.702783823013306</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.89677419354838706</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.97368421052631504</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" ref="G28:G30" si="6">(N3-F28)/N3*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>51.002341270446699</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.912903225806451</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.94736842105263097</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>53.158299684524501</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.90322580645161199</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30">
+        <v>0.89473684210526305</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="6"/>
+        <v>2.857142857142831</v>
       </c>
     </row>
   </sheetData>
@@ -3036,10 +4024,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D66360A-1272-4784-89D3-1A4D9D9015FE}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3106,7 +4094,7 @@
       </c>
       <c r="G2">
         <f>(N2-F2)/N2*100</f>
-        <v>22.222222222222271</v>
+        <v>26.315789473684305</v>
       </c>
       <c r="L2" t="s">
         <v>6</v>
@@ -3115,8 +4103,8 @@
         <v>12</v>
       </c>
       <c r="N2">
-        <f>MAX(F2, F7, F12, F17)</f>
-        <v>0.94736842105263097</v>
+        <f>MAX(F2, F7, F12, F17, F22, F27)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -3146,7 +4134,7 @@
         <v>11</v>
       </c>
       <c r="N3">
-        <f>MAX(F3, F8, F13, F18)</f>
+        <f>MAX(F3, F8, F13, F18, F23, F28)</f>
         <v>1</v>
       </c>
     </row>
@@ -3177,7 +4165,7 @@
         <v>8</v>
       </c>
       <c r="N4">
-        <f>MAX(F4, F9, F14, F19)</f>
+        <f t="shared" ref="N4:N5" si="1">MAX(F4, F9, F14, F19, F24, F29)</f>
         <v>1</v>
       </c>
     </row>
@@ -3208,7 +4196,7 @@
         <v>10</v>
       </c>
       <c r="N5">
-        <f>MAX(F5, F10, F15, F20)</f>
+        <f t="shared" si="1"/>
         <v>0.94736842105263097</v>
       </c>
     </row>
@@ -3251,12 +4239,12 @@
       <c r="E7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7">
         <v>0.94736842105263097</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7">
         <f>(N2-F7)/N2*100</f>
-        <v>0</v>
+        <v>5.2631578947369029</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -3276,7 +4264,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G10" si="1">(N3-F8)/N3*100</f>
+        <f t="shared" ref="G8:G10" si="2">(N3-F8)/N3*100</f>
         <v>0</v>
       </c>
     </row>
@@ -3297,7 +4285,7 @@
         <v>0.94736842105263097</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.2631578947369029</v>
       </c>
     </row>
@@ -3318,7 +4306,7 @@
         <v>0.89473684210526305</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.5555555555555056</v>
       </c>
     </row>
@@ -3366,7 +4354,7 @@
       </c>
       <c r="G12">
         <f>(N2-F12)/N2*100</f>
-        <v>5.5555555555555056</v>
+        <v>10.526315789473696</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
@@ -3386,7 +4374,7 @@
         <v>0.89473684210526305</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G15" si="2">(N3-F13)/N3*100</f>
+        <f t="shared" ref="G13:G15" si="3">(N3-F13)/N3*100</f>
         <v>10.526315789473696</v>
       </c>
     </row>
@@ -3407,7 +4395,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -3428,7 +4416,7 @@
         <v>0.84210526315789402</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11.11111111111113</v>
       </c>
     </row>
@@ -3471,12 +4459,12 @@
       <c r="E17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>0.94736842105263097</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17">
         <f>(N2-F17)/N2*100</f>
-        <v>0</v>
+        <v>5.2631578947369029</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -3496,7 +4484,7 @@
         <v>0.94736842105263097</v>
       </c>
       <c r="G18">
-        <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
+        <f t="shared" ref="G18:G20" si="4">(N3-F18)/N3*100</f>
         <v>5.2631578947369029</v>
       </c>
     </row>
@@ -3517,7 +4505,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -3538,7 +4526,203 @@
         <v>0.94736842105263097</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>(N2-F22)/N2*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G25" si="5">(N3-F23)/N3*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>593.49825525283802</v>
+      </c>
+      <c r="C27">
+        <v>0.99653379549393395</v>
+      </c>
+      <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <f>(N2-F27)/N2*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>467.72451424598597</v>
+      </c>
+      <c r="C28">
+        <v>0.99523396880415904</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" ref="G28:G30" si="6">(N3-F28)/N3*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>483.06091117858801</v>
+      </c>
+      <c r="C29">
+        <v>0.99610051993067505</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>528.79046154022205</v>
+      </c>
+      <c r="C30">
+        <v>0.99696707105719196</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.94736842105263097</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -3551,10 +4735,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3CDA24-B1F6-45D1-A3F6-E32FD37E9845}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3630,7 +4814,7 @@
         <v>12</v>
       </c>
       <c r="N2">
-        <f>MAX(F2, F7, F12, F17)</f>
+        <f>MAX(F2, F7, F12, F17, F22, F27)</f>
         <v>0.88333333333333297</v>
       </c>
     </row>
@@ -3661,7 +4845,7 @@
         <v>11</v>
       </c>
       <c r="N3">
-        <f>MAX(F3, F8, F13, F18)</f>
+        <f>MAX(F3, F8, F13, F18, F23, F28)</f>
         <v>0.86666666666666603</v>
       </c>
     </row>
@@ -3692,7 +4876,7 @@
         <v>8</v>
       </c>
       <c r="N4">
-        <f>MAX(F4, F9, F14, F19)</f>
+        <f t="shared" ref="N4:N5" si="1">MAX(F4, F9, F14, F19, F24, F29)</f>
         <v>0.96666666666666601</v>
       </c>
     </row>
@@ -3723,7 +4907,7 @@
         <v>10</v>
       </c>
       <c r="N5">
-        <f>MAX(F5, F10, F15, F20)</f>
+        <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
     </row>
@@ -3791,7 +4975,7 @@
         <v>0.78333333333333299</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G10" si="1">(N3-F8)/N3*100</f>
+        <f t="shared" ref="G8:G10" si="2">(N3-F8)/N3*100</f>
         <v>9.6153846153845883</v>
       </c>
     </row>
@@ -3812,7 +4996,7 @@
         <v>0.7</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27.58620689655168</v>
       </c>
     </row>
@@ -3833,7 +5017,7 @@
         <v>0.7</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.500000000000011</v>
       </c>
     </row>
@@ -3901,7 +5085,7 @@
         <v>0.86666666666666603</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" ref="G13:G15" si="2">(N3-F13)/N3*100</f>
+        <f t="shared" ref="G13:G15" si="3">(N3-F13)/N3*100</f>
         <v>0</v>
       </c>
     </row>
@@ -3922,7 +5106,7 @@
         <v>0.8</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17.241379310344769</v>
       </c>
     </row>
@@ -3943,7 +5127,7 @@
         <v>0.7</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12.500000000000011</v>
       </c>
     </row>
@@ -4011,7 +5195,7 @@
         <v>0</v>
       </c>
       <c r="G18">
-        <f t="shared" ref="G18:G20" si="3">(N3-F18)/N3*100</f>
+        <f t="shared" ref="G18:G20" si="4">(N3-F18)/N3*100</f>
         <v>100</v>
       </c>
     </row>
@@ -4032,7 +5216,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
@@ -4053,7 +5237,179 @@
         <v>0</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f>(N2-F22)/N2*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G25" si="5">(N3-F23)/N3*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <f>(N2-F27)/N2*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:G30" si="6">(N3-F28)/N3*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update PowerPoint & Excel
</commit_message>
<xml_diff>
--- a/Doc/Compare_Data.xlsx
+++ b/Doc/Compare_Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDF1EC2-D00A-455B-98AD-111AC07053E3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD3EC61-3523-5C41-BB5A-E1B5814E431B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12240" yWindow="5025" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cleveland_297" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="26">
   <si>
     <t>Validation</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -137,7 +138,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,26 +485,26 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F23" sqref="F23:G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="12.625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="18.125" customWidth="1"/>
-    <col min="8" max="8" width="10.375" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
     <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="11.625" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
-    <col min="14" max="14" width="10.625" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -535,7 +536,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -569,7 +570,7 @@
         <v>0.57195402298850495</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3">
         <v>1.39766025543212</v>
       </c>
@@ -600,7 +601,7 @@
         <v>0.61574712643678098</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4">
         <v>0.26223230361938399</v>
       </c>
@@ -631,7 +632,7 @@
         <v>0.58517241379310303</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5">
         <v>0.22420382499694799</v>
       </c>
@@ -662,7 +663,7 @@
         <v>0.58597701149425196</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -685,7 +686,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -709,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="B8">
         <v>109.103744029998</v>
       </c>
@@ -730,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="B9">
         <v>3.2319221496582</v>
       </c>
@@ -751,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="B10">
         <v>1.60746073722839</v>
       </c>
@@ -764,15 +765,15 @@
       <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>0.53252873563218395</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10">
         <f t="shared" si="2"/>
         <v>9.1212240094153092</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -795,7 +796,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -819,7 +820,7 @@
         <v>13.344051446945393</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="B13">
         <v>10.915215015411301</v>
       </c>
@@ -840,7 +841,7 @@
         <v>8.120216539107707</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="B14">
         <v>0.28925752639770502</v>
       </c>
@@ -861,7 +862,7 @@
         <v>2.8678059320368892</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="B15">
         <v>8.20744037628173E-2</v>
       </c>
@@ -882,7 +883,7 @@
         <v>10.906237740290232</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -905,7 +906,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -929,7 +930,7 @@
         <v>9.1840836012861971</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="B18">
         <v>13.047648191452</v>
       </c>
@@ -950,7 +951,7 @@
         <v>7.5788687698339183</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="B19">
         <v>0.274243354797363</v>
       </c>
@@ -971,7 +972,7 @@
         <v>5.1070516597917335</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="B20">
         <v>9.8088979721069294E-2</v>
       </c>
@@ -992,7 +993,7 @@
         <v>15.555119654766541</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1039,7 +1040,7 @@
         <v>7.0337620578777669</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="B23">
         <v>52.095729589462202</v>
       </c>
@@ -1060,7 +1061,7 @@
         <v>9.7815941758446492</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="B24">
         <v>1.04608631134033</v>
       </c>
@@ -1081,7 +1082,7 @@
         <v>1.0410528383422595</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="B25">
         <v>0.35929131507873502</v>
       </c>
@@ -1094,15 +1095,15 @@
       <c r="E25" t="s">
         <v>22</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>0.58597701149425196</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1125,7 +1126,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1149,7 +1150,7 @@
         <v>5.7676848874597342</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="B28">
         <v>2.2280247211456299</v>
       </c>
@@ -1170,7 +1171,7 @@
         <v>4.3494493186484462</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="B29">
         <v>2.23503065109252</v>
       </c>
@@ -1191,7 +1192,7 @@
         <v>6.8748772343350693</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="B30">
         <v>2.5012722015380802</v>
       </c>
@@ -1224,21 +1225,21 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="F30" sqref="F29:G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="15.875" customWidth="1"/>
-    <col min="4" max="4" width="13.125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" customWidth="1"/>
     <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="17.625" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1270,7 +1271,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1304,7 +1305,7 @@
         <v>0.90595238095238095</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3">
         <v>1.3984780311584399</v>
       </c>
@@ -1335,7 +1336,7 @@
         <v>0.89476190476190398</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4">
         <v>0.238202810287475</v>
       </c>
@@ -1366,7 +1367,7 @@
         <v>0.95158730158730098</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5">
         <v>0.24121904373168901</v>
       </c>
@@ -1397,7 +1398,7 @@
         <v>0.900555555555555</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1420,7 +1421,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1444,7 +1445,7 @@
         <v>1.2264564169951653</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="B8">
         <v>110.034425973892</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>3.1931878658860513</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="B9">
         <v>2.6844332218170099</v>
       </c>
@@ -1486,7 +1487,7 @@
         <v>1.7931609674728888</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="B10">
         <v>2.4071874618530198</v>
       </c>
@@ -1499,15 +1500,15 @@
       <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>0.89468253968253897</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10">
         <f t="shared" si="2"/>
         <v>0.65215475456069472</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1530,7 +1531,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1554,7 +1555,7 @@
         <v>2.4791940429260295</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="B13">
         <v>13.5132908821105</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>3.4858967535923173</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="B14">
         <v>0.18815779685974099</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>2.4186822351959893</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="B15">
         <v>0.226205348968505</v>
       </c>
@@ -1617,7 +1618,7 @@
         <v>2.5293028994448146</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1640,7 +1641,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1656,15 +1657,15 @@
       <c r="E17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>0.90309523809523795</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17">
         <f>(N2-F17)/N2*100</f>
         <v>0.3153745072273485</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="B18">
         <v>57.718045473098698</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="B19">
         <v>1.20709133148193</v>
       </c>
@@ -1706,7 +1707,7 @@
         <v>2.4020016680567324</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="B20">
         <v>1.39827013015747</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>2.2296642284304178</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1750,7 +1751,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1766,15 +1767,15 @@
       <c r="E22" t="s">
         <v>20</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>0.90595238095238095</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <f>(N2-F22)/N2*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="B23">
         <v>102.304795742034</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>4.7631718999467152</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="B24">
         <v>2.9672818183898899</v>
       </c>
@@ -1808,15 +1809,15 @@
       <c r="E24" t="s">
         <v>8</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>0.95158730158730098</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="B25">
         <v>1.87452912330627</v>
       </c>
@@ -1829,15 +1830,15 @@
       <c r="E25" t="s">
         <v>22</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>0.900555555555555</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1860,7 +1861,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1884,7 +1885,7 @@
         <v>0.91984231274645656</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="B28">
         <v>3.1728813648223801</v>
       </c>
@@ -1905,7 +1906,7 @@
         <v>2.5368103601205552</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="B29">
         <v>6.1375765800476003</v>
       </c>
@@ -1918,15 +1919,15 @@
       <c r="E29" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29">
         <v>0.94873015873015798</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29">
         <f t="shared" si="6"/>
         <v>0.30025020850710471</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="B30">
         <v>3.1418547630310001</v>
       </c>
@@ -1958,21 +1959,21 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="F27" sqref="F27:G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
-    <col min="4" max="4" width="14.375" customWidth="1"/>
-    <col min="5" max="5" width="11.875" customWidth="1"/>
-    <col min="6" max="6" width="14.625" customWidth="1"/>
-    <col min="7" max="7" width="12.875" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2020,10 +2021,10 @@
       <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2">
         <v>0.76666666666666605</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2">
         <f>(N2-F2)/N2*100</f>
         <v>1.4285714285714106</v>
       </c>
@@ -2038,7 +2039,7 @@
         <v>0.77777777777777701</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3">
         <v>1.2931752204895</v>
       </c>
@@ -2069,7 +2070,7 @@
         <v>0.844444444444444</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4">
         <v>0.139126300811767</v>
       </c>
@@ -2100,7 +2101,7 @@
         <v>0.84814814814814798</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5">
         <v>0.128116369247436</v>
       </c>
@@ -2131,7 +2132,7 @@
         <v>0.82222222222222197</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2154,7 +2155,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2178,7 +2179,7 @@
         <v>7.1428571428570811</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="B8">
         <v>109.446511745452</v>
       </c>
@@ -2199,7 +2200,7 @@
         <v>11.842105263157897</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="B9">
         <v>2.3251073360443102</v>
       </c>
@@ -2220,7 +2221,7 @@
         <v>9.1703056768559161</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="B10">
         <v>1.2781610488891599</v>
       </c>
@@ -2241,7 +2242,7 @@
         <v>12.612612612612647</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -2264,7 +2265,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2288,7 +2289,7 @@
         <v>1.904761904761938</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="B13">
         <v>14.2827265262603</v>
       </c>
@@ -2309,7 +2310,7 @@
         <v>5.7017543859649038</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="B14">
         <v>0.186163425445556</v>
       </c>
@@ -2330,7 +2331,7 @@
         <v>4.36681222707423</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="B15">
         <v>8.2066535949707003E-2</v>
       </c>
@@ -2351,7 +2352,7 @@
         <v>9.0090090090089969</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2374,7 +2375,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -2390,15 +2391,15 @@
       <c r="E17" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>0.76666666666666605</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17">
         <f>(N2-F17)/N2*100</f>
         <v>1.4285714285714106</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="B18">
         <v>19.015325069427401</v>
       </c>
@@ -2419,7 +2420,7 @@
         <v>1.7543859649122973</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="B19">
         <v>0.23221921920776301</v>
       </c>
@@ -2440,7 +2441,7 @@
         <v>0.87336244541491403</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="B20">
         <v>0.136123657226562</v>
       </c>
@@ -2453,15 +2454,15 @@
       <c r="E20" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20">
         <v>0.79629629629629595</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20">
         <f t="shared" si="4"/>
         <v>3.1531531531531654</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2484,7 +2485,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2500,15 +2501,15 @@
       <c r="E22" t="s">
         <v>20</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>0.77777777777777701</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="1">
         <f>(N2-F22)/N2*100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="B23">
         <v>96.969094753265296</v>
       </c>
@@ -2529,7 +2530,7 @@
         <v>5.7017543859649038</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="B24">
         <v>1.09184670448303</v>
       </c>
@@ -2550,7 +2551,7 @@
         <v>1.3100436681222534</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="B25">
         <v>0.45301771163940402</v>
       </c>
@@ -2563,15 +2564,15 @@
       <c r="E25" t="s">
         <v>22</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="1">
         <v>0.82222222222222197</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -2594,7 +2595,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2610,15 +2611,15 @@
       <c r="E27" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27">
         <v>0.76666666666666605</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27">
         <f>(N2-F27)/N2*100</f>
         <v>1.4285714285714106</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="B28">
         <v>1.87069988250732</v>
       </c>
@@ -2639,7 +2640,7 @@
         <v>3.5087719298246078</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="B29">
         <v>1.7976336479187001</v>
       </c>
@@ -2660,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="B30">
         <v>1.8406729698181099</v>
       </c>
@@ -2692,21 +2693,21 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="17.125" customWidth="1"/>
-    <col min="3" max="3" width="13.625" customWidth="1"/>
-    <col min="4" max="4" width="11.625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="16.125" customWidth="1"/>
-    <col min="7" max="7" width="16.375" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2738,7 +2739,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2772,7 +2773,7 @@
         <v>0.704397759103641</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3">
         <v>2.83370018005371</v>
       </c>
@@ -2803,7 +2804,7 @@
         <v>0.73053221288515402</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4">
         <v>1.4573731422424301</v>
       </c>
@@ -2834,7 +2835,7 @@
         <v>0.77184873949579802</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5">
         <v>1.37127161026</v>
       </c>
@@ -2865,7 +2866,7 @@
         <v>0.71264705882352897</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2888,7 +2889,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2912,11 +2913,11 @@
         <v>0.47719409869962892</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="B8">
         <v>113.07759594917199</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>0.44444444444444398</v>
       </c>
       <c r="D8" t="s">
@@ -2933,7 +2934,7 @@
         <v>4.2158742331288259</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="B9">
         <v>13.745487928390499</v>
       </c>
@@ -2954,7 +2955,7 @@
         <v>0.45726728361460478</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="B10">
         <v>5.3788866996765101</v>
       </c>
@@ -2975,7 +2976,7 @@
         <v>1.8198612503193485</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -2998,7 +2999,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3022,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="B13">
         <v>13.8055102825164</v>
       </c>
@@ -3043,7 +3044,7 @@
         <v>2.5977760736196989</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="B14">
         <v>1.1740648746490401</v>
       </c>
@@ -3064,7 +3065,7 @@
         <v>1.996007984031944</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="B15">
         <v>0.265232563018798</v>
       </c>
@@ -3085,7 +3086,7 @@
         <v>5.7838570838983507</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -3108,7 +3109,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3132,7 +3133,7 @@
         <v>3.1773173738417504</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="B18">
         <v>49.387864828109699</v>
       </c>
@@ -3153,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="B19">
         <v>3.8384819030761701</v>
       </c>
@@ -3174,7 +3175,7 @@
         <v>0.76029758664495295</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="B20">
         <v>0.892811298370361</v>
       </c>
@@ -3195,7 +3196,7 @@
         <v>3.6436530864925527</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -3218,7 +3219,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -3242,11 +3243,11 @@
         <v>1.1631606155803367</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="B23">
         <v>65.683366060256901</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>0.55555555555555503</v>
       </c>
       <c r="D23" t="s">
@@ -3263,7 +3264,7 @@
         <v>1.9401840490798725</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="B24">
         <v>6.5927386283874503</v>
       </c>
@@ -3284,7 +3285,7 @@
         <v>1.3736164035565794</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="B25">
         <v>1.99953269958496</v>
       </c>
@@ -3305,7 +3306,7 @@
         <v>1.6488807656781104</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -3328,7 +3329,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -3352,11 +3353,11 @@
         <v>1.3401200938481594</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="B28">
         <v>59.008615970611501</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>0.44444444444444398</v>
       </c>
       <c r="D28" t="s">
@@ -3373,7 +3374,7 @@
         <v>2.5958588957055642</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="B29">
         <v>62.341644048690704</v>
       </c>
@@ -3394,7 +3395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="B30">
         <v>103.141715049743</v>
       </c>
@@ -3426,22 +3427,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE6E0A8-C326-4938-968A-22A566DDA48F}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24:G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.375" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="14.125" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="16.375" customWidth="1"/>
-    <col min="7" max="7" width="11.875" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -3473,7 +3474,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3507,7 +3508,7 @@
         <v>0.94736842105263097</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3">
         <v>4.2344846725463796</v>
       </c>
@@ -3538,7 +3539,7 @@
         <v>0.97368421052631504</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4">
         <v>3.0740082263946502</v>
       </c>
@@ -3569,7 +3570,7 @@
         <v>0.94736842105263097</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5">
         <v>3.07286047935485</v>
       </c>
@@ -3600,7 +3601,7 @@
         <v>0.92105263157894701</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -3623,7 +3624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -3647,7 +3648,7 @@
         <v>16.666666666666647</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="B8">
         <v>111.56951546669001</v>
       </c>
@@ -3668,7 +3669,7 @@
         <v>43.243243243243242</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="B9">
         <v>3.8955338001251198</v>
       </c>
@@ -3689,7 +3690,7 @@
         <v>13.888888888888895</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="B10">
         <v>5.9524085521697998</v>
       </c>
@@ -3710,7 +3711,7 @@
         <v>8.5714285714286138</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -3733,7 +3734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3757,7 +3758,7 @@
         <v>11.11111111111113</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="B13">
         <v>13.8202545642852</v>
       </c>
@@ -3778,7 +3779,7 @@
         <v>5.4054054054053697</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="B14">
         <v>0.29825687408447199</v>
       </c>
@@ -3799,7 +3800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="B15">
         <v>0.408370971679687</v>
       </c>
@@ -3820,7 +3821,7 @@
         <v>2.857142857142831</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -3843,7 +3844,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3867,7 +3868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="B18">
         <v>870.95313930511395</v>
       </c>
@@ -3888,7 +3889,7 @@
         <v>2.7027027027026902</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="B19">
         <v>18.957506179809499</v>
       </c>
@@ -3909,7 +3910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="B20">
         <v>32.222971916198702</v>
       </c>
@@ -3930,7 +3931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -3953,7 +3954,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -3977,7 +3978,7 @@
         <v>2.7777777777777528</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="B23">
         <v>847.43173336982704</v>
       </c>
@@ -3998,7 +3999,7 @@
         <v>2.7027027027026902</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="B24">
         <v>99.745355129241901</v>
       </c>
@@ -4011,15 +4012,15 @@
       <c r="E24" t="s">
         <v>8</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="1">
         <v>0.94736842105263097</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="B25">
         <v>1.71541452407836</v>
       </c>
@@ -4040,7 +4041,7 @@
         <v>14.285714285714288</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -4063,7 +4064,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -4087,7 +4088,7 @@
         <v>2.7777777777777528</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="B28">
         <v>75.702783823013306</v>
       </c>
@@ -4108,7 +4109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="B29">
         <v>51.002341270446699</v>
       </c>
@@ -4129,7 +4130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="B30">
         <v>53.158299684524501</v>
       </c>
@@ -4160,22 +4161,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D66360A-1272-4784-89D3-1A4D9D9015FE}">
   <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
-    <col min="2" max="2" width="13.625" customWidth="1"/>
-    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="16.125" customWidth="1"/>
-    <col min="7" max="7" width="13.625" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4207,7 +4208,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -4241,7 +4242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3">
         <v>21.149477481841998</v>
       </c>
@@ -4272,7 +4273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="B4">
         <v>20.286529064178399</v>
       </c>
@@ -4303,7 +4304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="B5">
         <v>20.078588247299098</v>
       </c>
@@ -4334,7 +4335,7 @@
         <v>0.94736842105263097</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -4357,7 +4358,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -4381,7 +4382,7 @@
         <v>5.2631578947369029</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="B8">
         <v>113.038189649581</v>
       </c>
@@ -4402,7 +4403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="B9">
         <v>8.5047273635864205</v>
       </c>
@@ -4423,7 +4424,7 @@
         <v>5.2631578947369029</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="B10">
         <v>10.6006314754486</v>
       </c>
@@ -4444,7 +4445,7 @@
         <v>5.5555555555555056</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -4467,7 +4468,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -4491,7 +4492,7 @@
         <v>10.526315789473696</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="B13">
         <v>11.6274077892303</v>
       </c>
@@ -4512,7 +4513,7 @@
         <v>10.526315789473696</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14">
       <c r="B14">
         <v>1.3812491893768299</v>
       </c>
@@ -4533,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14">
       <c r="B15">
         <v>1.5153768062591499</v>
       </c>
@@ -4554,7 +4555,7 @@
         <v>11.11111111111113</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -4577,7 +4578,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -4601,7 +4602,7 @@
         <v>5.2631578947369029</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="B18">
         <v>6099.0280644893601</v>
       </c>
@@ -4622,7 +4623,7 @@
         <v>5.2631578947369029</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="B19">
         <v>561.18020677566506</v>
       </c>
@@ -4643,7 +4644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="B20">
         <v>711.095648050308</v>
       </c>
@@ -4664,7 +4665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -4687,7 +4688,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -4711,7 +4712,13 @@
         <v>10.526315789473696</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
       <c r="D23" t="s">
         <v>19</v>
       </c>
@@ -4726,7 +4733,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
       <c r="D24" t="s">
         <v>19</v>
       </c>
@@ -4741,7 +4754,13 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
       <c r="D25" t="s">
         <v>19</v>
       </c>
@@ -4756,7 +4775,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -4779,7 +4798,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -4803,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="B28">
         <v>467.72451424598597</v>
       </c>
@@ -4824,7 +4843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="B29">
         <v>483.06091117858801</v>
       </c>
@@ -4845,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="B30">
         <v>528.79046154022205</v>
       </c>
@@ -4878,21 +4897,21 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.875" customWidth="1"/>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="4" max="4" width="17.625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="14.375" customWidth="1"/>
-    <col min="7" max="7" width="12.125" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -4924,7 +4943,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -4958,7 +4977,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="B3">
         <v>379.95642280578602</v>
       </c>
@@ -4976,7 +4995,7 @@
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G5" si="0">(N3-F3)/N3*100</f>
-        <v>5.7692307692307789</v>
+        <v>15.517241379310356</v>
       </c>
       <c r="L3" t="s">
         <v>7</v>
@@ -4986,10 +5005,10 @@
       </c>
       <c r="N3">
         <f>MAX(F3, F8, F13, F18, F23, F28)</f>
-        <v>0.86666666666666603</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.96666666666666601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="B4">
         <v>422.91982841491699</v>
       </c>
@@ -5002,12 +5021,12 @@
       <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4">
         <v>0.96666666666666601</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6949152542373165</v>
       </c>
       <c r="L4" t="s">
         <v>7</v>
@@ -5017,10 +5036,10 @@
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N5" si="1">MAX(F4, F9, F14, F19, F24, F29)</f>
-        <v>0.96666666666666601</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>0.98333333333333295</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="B5">
         <v>375.75324440002402</v>
       </c>
@@ -5051,7 +5070,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -5074,7 +5093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -5098,7 +5117,7 @@
         <v>22.807017543859686</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="B8">
         <v>399.23260307312</v>
       </c>
@@ -5116,10 +5135,10 @@
       </c>
       <c r="G8">
         <f t="shared" ref="G8:G10" si="2">(N3-F8)/N3*100</f>
-        <v>9.6153846153845883</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>18.965517241379288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9">
         <v>338.36082291602997</v>
       </c>
@@ -5137,10 +5156,10 @@
       </c>
       <c r="G9">
         <f t="shared" si="2"/>
-        <v>27.58620689655168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>28.813559322033878</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="B10">
         <v>342.78976869583101</v>
       </c>
@@ -5161,7 +5180,7 @@
         <v>12.500000000000011</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -5184,7 +5203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -5208,7 +5227,7 @@
         <v>7.0175438596491571</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14">
       <c r="B13">
         <v>17.064989328384399</v>
       </c>
@@ -5221,15 +5240,15 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>0.86666666666666603</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13">
         <f t="shared" ref="G13:G15" si="3">(N3-F13)/N3*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>10.344827586206902</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="B14">
         <v>15.005628824234</v>
       </c>
@@ -5247,10 +5266,10 @@
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>17.241379310344769</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+        <v>18.644067796610134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="B15">
         <v>14.5131869316101</v>
       </c>
@@ -5271,7 +5290,7 @@
         <v>12.500000000000011</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -5294,7 +5313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5318,7 +5337,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="B18" t="s">
         <v>23</v>
       </c>
@@ -5339,7 +5358,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="B19" t="s">
         <v>23</v>
       </c>
@@ -5360,7 +5379,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -5381,7 +5400,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -5404,12 +5423,18 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>24</v>
       </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s">
         <v>20</v>
@@ -5422,9 +5447,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E23" t="s">
         <v>11</v>
@@ -5437,9 +5468,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -5452,9 +5489,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E25" t="s">
         <v>22</v>
@@ -5467,7 +5510,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -5490,7 +5533,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -5501,7 +5544,7 @@
         <v>0.98619999999999997</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E27" t="s">
         <v>20</v>
@@ -5514,49 +5557,67 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
+      <c r="B28">
+        <v>7478.9689521789496</v>
+      </c>
+      <c r="C28">
+        <v>0.98919999999999997</v>
+      </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E28" t="s">
         <v>11</v>
       </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
+      <c r="F28" s="1">
+        <v>0.96666666666666601</v>
+      </c>
+      <c r="G28" s="1">
         <f t="shared" ref="G28:G30" si="6">(N3-F28)/N3*100</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="B29">
+        <v>4854.7832219600596</v>
+      </c>
+      <c r="C29">
+        <v>0.98939999999999995</v>
+      </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E29" t="s">
         <v>8</v>
       </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-      <c r="G29">
+      <c r="F29" s="1">
+        <v>0.98333333333333295</v>
+      </c>
+      <c r="G29" s="1">
         <f t="shared" si="6"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30">
+        <v>4824.5435917377399</v>
+      </c>
+      <c r="C30">
+        <v>0.97770000000000001</v>
+      </c>
       <c r="D30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E30" t="s">
         <v>22</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>0.71666666666666601</v>
       </c>
       <c r="G30">
         <f t="shared" si="6"/>
-        <v>100</v>
+        <v>10.416666666666755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>